<commit_message>
updated spreadsheet with to include power factor variables
</commit_message>
<xml_diff>
--- a/CaseStudies/SimulinkOpal/Device_Integration_Test_01_OpalReady_v3/UDP Data Format - Device Integration Test 01.xlsx
+++ b/CaseStudies/SimulinkOpal/Device_Integration_Test_01_OpalReady_v3/UDP Data Format - Device Integration Test 01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Waveform</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Misc Data Set#2</t>
   </si>
   <si>
-    <t>PF</t>
-  </si>
-  <si>
     <t>on/off</t>
   </si>
   <si>
@@ -169,16 +166,22 @@
     <t>Misc Data</t>
   </si>
   <si>
-    <t>Misc Data Set#3</t>
-  </si>
-  <si>
-    <t>int17</t>
-  </si>
-  <si>
     <t>Btu/Hr, and degree F</t>
   </si>
   <si>
     <t>VRMSLL, Hz, degrees-angle</t>
+  </si>
+  <si>
+    <t>Power Factor Data</t>
+  </si>
+  <si>
+    <t>Power Factor</t>
+  </si>
+  <si>
+    <t>Import/Export</t>
+  </si>
+  <si>
+    <t>Lagging/Leading</t>
   </si>
 </sst>
 </file>
@@ -617,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1</v>
@@ -703,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F4:F19" si="0">RIGHT(C4,2)/8*D4*E4*$C$1</f>
+        <f t="shared" ref="F4:F21" si="0">RIGHT(C4,2)/8*D4*E4*$C$1</f>
         <v>10</v>
       </c>
       <c r="G4" s="6"/>
@@ -716,7 +719,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -747,7 +750,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -777,7 +780,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -807,7 +810,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -837,7 +840,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -867,7 +870,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -939,7 +942,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -956,7 +959,7 @@
       </c>
       <c r="I13" s="3"/>
       <c r="K13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -983,10 +986,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1001,218 +1004,257 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H15" s="4"/>
       <c r="I15" s="3">
         <v>1000</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="12" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>63.75</v>
-      </c>
-      <c r="H16" s="4"/>
+        <v>10</v>
+      </c>
       <c r="I16" s="3">
-        <v>100</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="12" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3">
+        <v>100</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I19" s="3">
+        <v>10</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="I17" s="3">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="K19" s="13" t="s">
+      <c r="I21" s="4"/>
+      <c r="K21" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <f>SUM(E6:E19)+E4+D5*E5</f>
-        <v>532</v>
-      </c>
-    </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="s">
+      <c r="E22">
+        <f>SUM(E6:E21)+E4+D5*E5</f>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
-        <f>SUM(F4:F21)</f>
-        <v>5323.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1">
+        <f>SUM(F4:F23)</f>
+        <v>5340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C25" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F26" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="1"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="18">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="18">
-        <v>2</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>28</v>
-      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="1"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="2"/>
+      <c r="F27" s="18">
+        <v>1</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1226,6 +1268,12 @@
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>